<commit_message>
Translate inline comments in index.html to Chinese; fix avatar tilt/recovery and hover/animation conflicts.
Translate inline comments in index.html to Chinese; fix avatar tilt/recovery and hover/animation conflicts.
</commit_message>
<xml_diff>
--- a/nicknames.xlsx
+++ b/nicknames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\文档\GitHub\Lucky-Draw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA22FDD-E28A-4EC2-85D4-B0F647EF8E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E995C074-0E00-4192-9EEE-A76C3C11D36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3375" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,10 +132,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Tachibana Kousuke</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>艾炜杰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -195,10 +191,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>情商巅峰时期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>无恙.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -451,9 +443,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://pic1.imgdb.cn/item/6932847ed1e741a32bf1ba01.jpg</t>
-  </si>
-  <si>
     <t>https://pic1.imgdb.cn/item/69328489d1e741a32bf1ba12.jpg</t>
   </si>
   <si>
@@ -575,10 +564,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>何亦嘉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>刘知易</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -586,10 +571,6 @@
     <t>政治</t>
   </si>
   <si>
-    <t>青+A2:A52行归</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">政治 </t>
   </si>
   <si>
@@ -605,6 +586,26 @@
   </si>
   <si>
     <t>分科</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青行归</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PhuDgue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>何奕嘉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Takion Kroslin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://pic1.imgdb.cn/item/694fe8e5161224305eb30b3e.jpg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -697,7 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -708,7 +709,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -992,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="139" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1012,736 +1012,736 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>162</v>
+      <c r="D1" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>156</v>
+        <v>102</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>159</v>
+        <v>100</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>156</v>
+        <v>104</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>159</v>
+        <v>108</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>159</v>
+        <v>107</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>159</v>
+        <v>106</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>159</v>
+        <v>105</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>156</v>
+        <v>109</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>159</v>
+        <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>159</v>
+        <v>111</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>156</v>
+        <v>110</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>159</v>
+        <v>112</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>159</v>
+        <v>113</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>159</v>
+        <v>114</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>159</v>
+        <v>117</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>159</v>
+      <c r="C20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>159</v>
+        <v>116</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>159</v>
+        <v>115</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>159</v>
+        <v>120</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>156</v>
+        <v>118</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>156</v>
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>159</v>
+        <v>121</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>159</v>
+        <v>119</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>156</v>
+        <v>127</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>159</v>
+        <v>148</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>156</v>
+        <v>126</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>159</v>
+        <v>125</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>159</v>
+        <v>124</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>159</v>
+        <v>123</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>159</v>
+        <v>129</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>159</v>
+        <v>128</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>159</v>
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>159</v>
+        <v>132</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>156</v>
+        <v>137</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>159</v>
+        <v>135</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>156</v>
+        <v>134</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>159</v>
+        <v>136</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>159</v>
+        <v>133</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>156</v>
+        <v>142</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>159</v>
+        <v>139</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>159</v>
+        <v>141</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>159</v>
+        <v>138</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>156</v>
+        <v>140</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>159</v>
+        <v>145</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>159</v>
+        <v>143</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>159</v>
+        <v>146</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>159</v>
+        <v>144</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B53" s="8" t="s">
         <v>155</v>
       </c>
+      <c r="B53" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="C53" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1785,8 +1785,9 @@
     <hyperlink ref="C49" r:id="rId33" xr:uid="{203F949A-E3A9-4C52-A3C3-FCCE9853C533}"/>
     <hyperlink ref="C17" r:id="rId34" xr:uid="{8B3BCAFF-F9CF-407C-A3D8-CF730573F938}"/>
     <hyperlink ref="C53" r:id="rId35" xr:uid="{5449CF26-59BF-405A-BBE7-163AA95C1089}"/>
+    <hyperlink ref="C20" r:id="rId36" xr:uid="{2BE7D7DD-CA4F-48F5-9FE3-10374996C2A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>